<commit_message>
updates to switch easily to vodites
</commit_message>
<xml_diff>
--- a/Exports/TeamExport_A46051_Alpha_M_Period 5.xlsx
+++ b/Exports/TeamExport_A46051_Alpha_M_Period 5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Anno III\UCSD\112\Markstrat\Code\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4A22A1-48B3-4BF1-BE95-2F3589BFFF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0FE8D1-B349-4219-BE5A-4854D7EFBE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Firm" sheetId="1" r:id="rId1"/>
@@ -2453,19 +2453,19 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5834,8 +5834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8075,7 +8075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O592"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A216" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A216" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I223" sqref="I223"/>
     </sheetView>
   </sheetViews>
@@ -16575,21 +16575,21 @@
     </row>
     <row r="551" spans="1:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B551" s="9"/>
-      <c r="F551" s="329" t="s">
+      <c r="F551" s="327" t="s">
         <v>191</v>
       </c>
-      <c r="G551" s="330"/>
-      <c r="H551" s="331"/>
-      <c r="I551" s="329" t="s">
+      <c r="G551" s="328"/>
+      <c r="H551" s="329"/>
+      <c r="I551" s="327" t="s">
         <v>192</v>
       </c>
-      <c r="J551" s="330"/>
-      <c r="K551" s="331"/>
-      <c r="L551" s="329" t="s">
+      <c r="J551" s="328"/>
+      <c r="K551" s="329"/>
+      <c r="L551" s="327" t="s">
         <v>193</v>
       </c>
-      <c r="M551" s="330"/>
-      <c r="N551" s="331"/>
+      <c r="M551" s="328"/>
+      <c r="N551" s="329"/>
     </row>
     <row r="552" spans="1:14" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B552" s="82"/>
@@ -17023,22 +17023,22 @@
     <row r="571" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A571" s="3"/>
       <c r="B571" s="9"/>
-      <c r="F571" s="327" t="s">
+      <c r="F571" s="330" t="s">
         <v>201</v>
       </c>
-      <c r="G571" s="328"/>
-      <c r="H571" s="327" t="s">
+      <c r="G571" s="331"/>
+      <c r="H571" s="330" t="s">
         <v>203</v>
       </c>
-      <c r="I571" s="328"/>
-      <c r="J571" s="327" t="s">
+      <c r="I571" s="331"/>
+      <c r="J571" s="330" t="s">
         <v>113</v>
       </c>
-      <c r="K571" s="328"/>
-      <c r="L571" s="327" t="s">
+      <c r="K571" s="331"/>
+      <c r="L571" s="330" t="s">
         <v>147</v>
       </c>
-      <c r="M571" s="328"/>
+      <c r="M571" s="331"/>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A572" s="3"/>
@@ -17671,34 +17671,34 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="L571:M571"/>
+    <mergeCell ref="F571:G571"/>
+    <mergeCell ref="H571:I571"/>
+    <mergeCell ref="J571:K571"/>
+    <mergeCell ref="D563:E563"/>
+    <mergeCell ref="L551:N551"/>
+    <mergeCell ref="D515:E515"/>
+    <mergeCell ref="D525:E525"/>
+    <mergeCell ref="D533:E533"/>
+    <mergeCell ref="D541:E541"/>
+    <mergeCell ref="J187:M187"/>
+    <mergeCell ref="D152:E153"/>
+    <mergeCell ref="F152:I152"/>
+    <mergeCell ref="J152:M152"/>
+    <mergeCell ref="D362:E362"/>
+    <mergeCell ref="D187:E188"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="D82:E82"/>
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="D572:E572"/>
     <mergeCell ref="F187:I187"/>
-    <mergeCell ref="J187:M187"/>
-    <mergeCell ref="D152:E153"/>
-    <mergeCell ref="F152:I152"/>
-    <mergeCell ref="J152:M152"/>
-    <mergeCell ref="D362:E362"/>
     <mergeCell ref="D372:E372"/>
-    <mergeCell ref="D187:E188"/>
     <mergeCell ref="D552:E552"/>
     <mergeCell ref="D454:E454"/>
     <mergeCell ref="D499:E499"/>
     <mergeCell ref="D507:E507"/>
     <mergeCell ref="F551:H551"/>
     <mergeCell ref="I551:K551"/>
-    <mergeCell ref="L551:N551"/>
-    <mergeCell ref="D515:E515"/>
-    <mergeCell ref="D525:E525"/>
-    <mergeCell ref="D533:E533"/>
-    <mergeCell ref="D541:E541"/>
-    <mergeCell ref="L571:M571"/>
-    <mergeCell ref="F571:G571"/>
-    <mergeCell ref="H571:I571"/>
-    <mergeCell ref="J571:K571"/>
-    <mergeCell ref="D563:E563"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24290,21 +24290,21 @@
     </row>
     <row r="551" spans="1:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B551" s="9"/>
-      <c r="F551" s="329" t="s">
+      <c r="F551" s="327" t="s">
         <v>191</v>
       </c>
-      <c r="G551" s="330"/>
-      <c r="H551" s="331"/>
-      <c r="I551" s="329" t="s">
+      <c r="G551" s="328"/>
+      <c r="H551" s="329"/>
+      <c r="I551" s="327" t="s">
         <v>192</v>
       </c>
-      <c r="J551" s="330"/>
-      <c r="K551" s="331"/>
-      <c r="L551" s="329" t="s">
+      <c r="J551" s="328"/>
+      <c r="K551" s="329"/>
+      <c r="L551" s="327" t="s">
         <v>193</v>
       </c>
-      <c r="M551" s="330"/>
-      <c r="N551" s="331"/>
+      <c r="M551" s="328"/>
+      <c r="N551" s="329"/>
     </row>
     <row r="552" spans="1:14" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B552" s="82"/>
@@ -24690,22 +24690,22 @@
     <row r="571" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A571" s="3"/>
       <c r="B571" s="9"/>
-      <c r="F571" s="327" t="s">
+      <c r="F571" s="330" t="s">
         <v>147</v>
       </c>
-      <c r="G571" s="328"/>
-      <c r="H571" s="327" t="s">
+      <c r="G571" s="331"/>
+      <c r="H571" s="330" t="s">
         <v>78</v>
       </c>
-      <c r="I571" s="328"/>
-      <c r="J571" s="327" t="s">
+      <c r="I571" s="331"/>
+      <c r="J571" s="330" t="s">
         <v>224</v>
       </c>
-      <c r="K571" s="328"/>
-      <c r="L571" s="327" t="s">
+      <c r="K571" s="331"/>
+      <c r="L571" s="330" t="s">
         <v>120</v>
       </c>
-      <c r="M571" s="328"/>
+      <c r="M571" s="331"/>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A572" s="3"/>
@@ -25206,6 +25206,33 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="D362:E362"/>
+    <mergeCell ref="D372:E372"/>
+    <mergeCell ref="D187:E188"/>
+    <mergeCell ref="F187:I187"/>
+    <mergeCell ref="J187:M187"/>
+    <mergeCell ref="D223:E223"/>
+    <mergeCell ref="D296:E296"/>
+    <mergeCell ref="D152:E153"/>
+    <mergeCell ref="F152:I152"/>
+    <mergeCell ref="J152:M152"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D383:E383"/>
+    <mergeCell ref="D454:E454"/>
+    <mergeCell ref="D464:E464"/>
+    <mergeCell ref="D499:E499"/>
+    <mergeCell ref="D507:E507"/>
+    <mergeCell ref="D418:E418"/>
+    <mergeCell ref="D515:E515"/>
+    <mergeCell ref="D525:E525"/>
+    <mergeCell ref="D533:E533"/>
+    <mergeCell ref="F551:H551"/>
+    <mergeCell ref="I551:K551"/>
+    <mergeCell ref="D541:E541"/>
     <mergeCell ref="D572:E572"/>
     <mergeCell ref="L551:N551"/>
     <mergeCell ref="D552:E552"/>
@@ -25214,33 +25241,6 @@
     <mergeCell ref="H571:I571"/>
     <mergeCell ref="J571:K571"/>
     <mergeCell ref="L571:M571"/>
-    <mergeCell ref="D515:E515"/>
-    <mergeCell ref="D525:E525"/>
-    <mergeCell ref="D533:E533"/>
-    <mergeCell ref="F551:H551"/>
-    <mergeCell ref="I551:K551"/>
-    <mergeCell ref="D541:E541"/>
-    <mergeCell ref="D383:E383"/>
-    <mergeCell ref="D454:E454"/>
-    <mergeCell ref="D464:E464"/>
-    <mergeCell ref="D499:E499"/>
-    <mergeCell ref="D507:E507"/>
-    <mergeCell ref="D418:E418"/>
-    <mergeCell ref="D152:E153"/>
-    <mergeCell ref="F152:I152"/>
-    <mergeCell ref="J152:M152"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D362:E362"/>
-    <mergeCell ref="D372:E372"/>
-    <mergeCell ref="D187:E188"/>
-    <mergeCell ref="F187:I187"/>
-    <mergeCell ref="J187:M187"/>
-    <mergeCell ref="D223:E223"/>
-    <mergeCell ref="D296:E296"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>